<commit_message>
revised version; first release
</commit_message>
<xml_diff>
--- a/exampleMinimal.xlsx
+++ b/exampleMinimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronste\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88332269-2262-4979-BB41-B09A91FB468E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0423F4-5319-49DF-ABDC-FAD230DE8D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,24 +39,6 @@
     <t>sectionAbbrev</t>
   </si>
   <si>
-    <t>pages</t>
-  </si>
-  <si>
-    <t>authorFirstname1</t>
-  </si>
-  <si>
-    <t>authorLastname2</t>
-  </si>
-  <si>
-    <t>authorLastname1</t>
-  </si>
-  <si>
-    <t>file1</t>
-  </si>
-  <si>
-    <t>authorFirstname2</t>
-  </si>
-  <si>
     <t>fileGenre1</t>
   </si>
   <si>
@@ -81,9 +63,6 @@
     <t>PDF</t>
   </si>
   <si>
-    <t>fileLabel1</t>
-  </si>
-  <si>
     <t>2017-1-1-1.pdf</t>
   </si>
   <si>
@@ -114,12 +93,6 @@
     <t>en</t>
   </si>
   <si>
-    <t>fileLocale1</t>
-  </si>
-  <si>
-    <t>seq</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -163,6 +136,33 @@
   </si>
   <si>
     <t>issueDatePublished</t>
+  </si>
+  <si>
+    <t>articlePages</t>
+  </si>
+  <si>
+    <t>articleSeq</t>
+  </si>
+  <si>
+    <t>fileName1</t>
+  </si>
+  <si>
+    <t>authorGivenname1</t>
+  </si>
+  <si>
+    <t>authorFamilyname1</t>
+  </si>
+  <si>
+    <t>authorGivenname2</t>
+  </si>
+  <si>
+    <t>authorFamilyname2</t>
+  </si>
+  <si>
+    <t>galleyLabel1</t>
+  </si>
+  <si>
+    <t>galleyLocale1</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -535,10 +535,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -550,42 +550,42 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5">
         <v>42808</v>
@@ -594,48 +594,48 @@
         <v>2017</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="L2" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5">
         <v>42808</v>
@@ -644,42 +644,42 @@
         <v>2017</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5">
         <v>43250</v>
@@ -688,42 +688,42 @@
         <v>2018</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5">
         <v>43250</v>
@@ -732,34 +732,34 @@
         <v>2018</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>